<commit_message>
Updated Hours for Mike/Patrick
Also marked PDF as original and not live or active, since we use the live link now.
</commit_message>
<xml_diff>
--- a/Time Sheet.xlsx
+++ b/Time Sheet.xlsx
@@ -174,7 +174,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -241,13 +241,19 @@
         <f aca="false">B4</f>
         <v>2</v>
       </c>
+      <c r="D4" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="E4" s="0" t="n">
         <f aca="false">D4</f>
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>2</v>
       </c>
       <c r="G4" s="0" t="n">
         <f aca="false">F4</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I4" s="0" t="n">
         <f aca="false">H4</f>
@@ -264,7 +270,7 @@
       </c>
       <c r="E5" s="0" t="n">
         <f aca="false">D5+E4</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G5" s="0" t="n">
         <f aca="false">F5</f>
@@ -285,7 +291,7 @@
       </c>
       <c r="E6" s="0" t="n">
         <f aca="false">D6+E5</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G6" s="0" t="n">
         <f aca="false">F6</f>
@@ -306,7 +312,7 @@
       </c>
       <c r="E7" s="0" t="n">
         <f aca="false">D7+E6</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G7" s="0" t="n">
         <f aca="false">F7</f>
@@ -327,7 +333,7 @@
       </c>
       <c r="E8" s="0" t="n">
         <f aca="false">D8+E7</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G8" s="0" t="n">
         <f aca="false">F8</f>
@@ -348,7 +354,7 @@
       </c>
       <c r="E9" s="0" t="n">
         <f aca="false">D9+E8</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G9" s="0" t="n">
         <f aca="false">F9</f>
@@ -369,7 +375,7 @@
       </c>
       <c r="E10" s="0" t="n">
         <f aca="false">D10+E9</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G10" s="0" t="n">
         <f aca="false">F10</f>
@@ -390,7 +396,7 @@
       </c>
       <c r="E11" s="0" t="n">
         <f aca="false">D11+E10</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G11" s="0" t="n">
         <f aca="false">F11</f>
@@ -411,7 +417,7 @@
       </c>
       <c r="E12" s="0" t="n">
         <f aca="false">D12+E11</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G12" s="0" t="n">
         <f aca="false">F12</f>
@@ -432,7 +438,7 @@
       </c>
       <c r="E13" s="0" t="n">
         <f aca="false">D13+E12</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G13" s="0" t="n">
         <f aca="false">F13</f>

</xml_diff>

<commit_message>
Updated times for week
Updated times for patrick and mike
</commit_message>
<xml_diff>
--- a/Time Sheet.xlsx
+++ b/Time Sheet.xlsx
@@ -174,7 +174,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -242,18 +242,18 @@
         <v>4</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E4" s="0" t="n">
         <f aca="false">D4</f>
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>7.5</v>
+        <v>13.5</v>
       </c>
       <c r="G4" s="0" t="n">
         <f aca="false">F4</f>
-        <v>7.5</v>
+        <v>13.5</v>
       </c>
       <c r="I4" s="0" t="n">
         <f aca="false">H4</f>
@@ -268,13 +268,19 @@
         <f aca="false">B5+C4</f>
         <v>4</v>
       </c>
+      <c r="D5" s="0" t="n">
+        <v>13</v>
+      </c>
       <c r="E5" s="0" t="n">
         <f aca="false">D5+E4</f>
-        <v>8</v>
+        <v>28</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>13</v>
       </c>
       <c r="G5" s="0" t="n">
         <f aca="false">F5</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="I5" s="0" t="n">
         <f aca="false">H5</f>
@@ -291,7 +297,7 @@
       </c>
       <c r="E6" s="0" t="n">
         <f aca="false">D6+E5</f>
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="G6" s="0" t="n">
         <f aca="false">F6</f>
@@ -312,7 +318,7 @@
       </c>
       <c r="E7" s="0" t="n">
         <f aca="false">D7+E6</f>
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="G7" s="0" t="n">
         <f aca="false">F7</f>
@@ -333,7 +339,7 @@
       </c>
       <c r="E8" s="0" t="n">
         <f aca="false">D8+E7</f>
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="G8" s="0" t="n">
         <f aca="false">F8</f>
@@ -354,7 +360,7 @@
       </c>
       <c r="E9" s="0" t="n">
         <f aca="false">D9+E8</f>
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="G9" s="0" t="n">
         <f aca="false">F9</f>
@@ -375,7 +381,7 @@
       </c>
       <c r="E10" s="0" t="n">
         <f aca="false">D10+E9</f>
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="G10" s="0" t="n">
         <f aca="false">F10</f>
@@ -396,7 +402,7 @@
       </c>
       <c r="E11" s="0" t="n">
         <f aca="false">D11+E10</f>
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="G11" s="0" t="n">
         <f aca="false">F11</f>
@@ -417,7 +423,7 @@
       </c>
       <c r="E12" s="0" t="n">
         <f aca="false">D12+E11</f>
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="G12" s="0" t="n">
         <f aca="false">F12</f>
@@ -438,7 +444,7 @@
       </c>
       <c r="E13" s="0" t="n">
         <f aca="false">D13+E12</f>
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="G13" s="0" t="n">
         <f aca="false">F13</f>

</xml_diff>

<commit_message>
Hyrum added time for last week
Sorry I've haven't been so productive!
</commit_message>
<xml_diff>
--- a/Time Sheet.xlsx
+++ b/Time Sheet.xlsx
@@ -173,8 +173,8 @@
   </sheetPr>
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -264,9 +264,12 @@
       <c r="A5" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="B5" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="C5" s="0" t="n">
         <f aca="false">B5+C4</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>13</v>
@@ -293,7 +296,7 @@
       </c>
       <c r="C6" s="0" t="n">
         <f aca="false">B6+C5</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E6" s="0" t="n">
         <f aca="false">D6+E5</f>
@@ -314,7 +317,7 @@
       </c>
       <c r="C7" s="0" t="n">
         <f aca="false">B7+C6</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E7" s="0" t="n">
         <f aca="false">D7+E6</f>
@@ -335,7 +338,7 @@
       </c>
       <c r="C8" s="0" t="n">
         <f aca="false">B8+C7</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E8" s="0" t="n">
         <f aca="false">D8+E7</f>
@@ -356,7 +359,7 @@
       </c>
       <c r="C9" s="0" t="n">
         <f aca="false">B9+C8</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E9" s="0" t="n">
         <f aca="false">D9+E8</f>
@@ -377,7 +380,7 @@
       </c>
       <c r="C10" s="0" t="n">
         <f aca="false">B10+C9</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E10" s="0" t="n">
         <f aca="false">D10+E9</f>
@@ -398,7 +401,7 @@
       </c>
       <c r="C11" s="0" t="n">
         <f aca="false">B11+C10</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E11" s="0" t="n">
         <f aca="false">D11+E10</f>
@@ -419,7 +422,7 @@
       </c>
       <c r="C12" s="0" t="n">
         <f aca="false">B12+C11</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E12" s="0" t="n">
         <f aca="false">D12+E11</f>
@@ -440,7 +443,7 @@
       </c>
       <c r="C13" s="0" t="n">
         <f aca="false">B13+C12</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E13" s="0" t="n">
         <f aca="false">D13+E12</f>

</xml_diff>

<commit_message>
Added hours for week 3
</commit_message>
<xml_diff>
--- a/Time Sheet.xlsx
+++ b/Time Sheet.xlsx
@@ -173,8 +173,8 @@
   </sheetPr>
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -282,8 +282,8 @@
         <v>13</v>
       </c>
       <c r="G5" s="0" t="n">
-        <f aca="false">F5</f>
-        <v>13</v>
+        <f aca="false">F5 +G4</f>
+        <v>26.5</v>
       </c>
       <c r="I5" s="0" t="n">
         <f aca="false">H5</f>
@@ -294,9 +294,12 @@
       <c r="A6" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="B6" s="0" t="n">
+        <v>9</v>
+      </c>
       <c r="C6" s="0" t="n">
         <f aca="false">B6+C5</f>
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>13</v>
@@ -309,8 +312,8 @@
         <v>8</v>
       </c>
       <c r="G6" s="0" t="n">
-        <f aca="false">F6</f>
-        <v>8</v>
+        <f aca="false">F6 + G5</f>
+        <v>34.5</v>
       </c>
       <c r="I6" s="0" t="n">
         <f aca="false">H6</f>
@@ -323,15 +326,15 @@
       </c>
       <c r="C7" s="0" t="n">
         <f aca="false">B7+C6</f>
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E7" s="0" t="n">
         <f aca="false">D7+E6</f>
         <v>41</v>
       </c>
       <c r="G7" s="0" t="n">
-        <f aca="false">F7</f>
-        <v>0</v>
+        <f aca="false">F7 +G6</f>
+        <v>34.5</v>
       </c>
       <c r="I7" s="0" t="n">
         <f aca="false">H7</f>
@@ -344,15 +347,15 @@
       </c>
       <c r="C8" s="0" t="n">
         <f aca="false">B8+C7</f>
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E8" s="0" t="n">
         <f aca="false">D8+E7</f>
         <v>41</v>
       </c>
       <c r="G8" s="0" t="n">
-        <f aca="false">F8</f>
-        <v>0</v>
+        <f aca="false">F8+G7</f>
+        <v>34.5</v>
       </c>
       <c r="I8" s="0" t="n">
         <f aca="false">H8</f>
@@ -365,15 +368,15 @@
       </c>
       <c r="C9" s="0" t="n">
         <f aca="false">B9+C8</f>
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E9" s="0" t="n">
         <f aca="false">D9+E8</f>
         <v>41</v>
       </c>
       <c r="G9" s="0" t="n">
-        <f aca="false">F9</f>
-        <v>0</v>
+        <f aca="false">F9 +G8</f>
+        <v>34.5</v>
       </c>
       <c r="I9" s="0" t="n">
         <f aca="false">H9</f>
@@ -386,15 +389,15 @@
       </c>
       <c r="C10" s="0" t="n">
         <f aca="false">B10+C9</f>
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E10" s="0" t="n">
         <f aca="false">D10+E9</f>
         <v>41</v>
       </c>
       <c r="G10" s="0" t="n">
-        <f aca="false">F10</f>
-        <v>0</v>
+        <f aca="false">F10 +G9</f>
+        <v>34.5</v>
       </c>
       <c r="I10" s="0" t="n">
         <f aca="false">H10</f>
@@ -407,36 +410,36 @@
       </c>
       <c r="C11" s="0" t="n">
         <f aca="false">B11+C10</f>
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E11" s="0" t="n">
         <f aca="false">D11+E10</f>
         <v>41</v>
       </c>
       <c r="G11" s="0" t="n">
-        <f aca="false">F11</f>
-        <v>0</v>
+        <f aca="false">F11+G10</f>
+        <v>34.5</v>
       </c>
       <c r="I11" s="0" t="n">
         <f aca="false">H11</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>16</v>
       </c>
       <c r="C12" s="0" t="n">
         <f aca="false">B12+C11</f>
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E12" s="0" t="n">
         <f aca="false">D12+E11</f>
         <v>41</v>
       </c>
       <c r="G12" s="0" t="n">
-        <f aca="false">F12</f>
-        <v>0</v>
+        <f aca="false">F12+G11</f>
+        <v>34.5</v>
       </c>
       <c r="I12" s="0" t="n">
         <f aca="false">H12</f>
@@ -449,15 +452,15 @@
       </c>
       <c r="C13" s="0" t="n">
         <f aca="false">B13+C12</f>
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E13" s="0" t="n">
         <f aca="false">D13+E12</f>
         <v>41</v>
       </c>
       <c r="G13" s="0" t="n">
-        <f aca="false">F13</f>
-        <v>0</v>
+        <f aca="false">F13+G12</f>
+        <v>34.5</v>
       </c>
       <c r="I13" s="0" t="n">
         <f aca="false">H13</f>

</xml_diff>

<commit_message>
Added week 4 time
</commit_message>
<xml_diff>
--- a/Time Sheet.xlsx
+++ b/Time Sheet.xlsx
@@ -174,7 +174,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -324,9 +324,12 @@
       <c r="A7" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="B7" s="0" t="n">
+        <v>10</v>
+      </c>
       <c r="C7" s="0" t="n">
         <f aca="false">B7+C6</f>
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E7" s="0" t="n">
         <f aca="false">D7+E6</f>
@@ -347,7 +350,7 @@
       </c>
       <c r="C8" s="0" t="n">
         <f aca="false">B8+C7</f>
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E8" s="0" t="n">
         <f aca="false">D8+E7</f>
@@ -368,7 +371,7 @@
       </c>
       <c r="C9" s="0" t="n">
         <f aca="false">B9+C8</f>
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E9" s="0" t="n">
         <f aca="false">D9+E8</f>
@@ -389,7 +392,7 @@
       </c>
       <c r="C10" s="0" t="n">
         <f aca="false">B10+C9</f>
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E10" s="0" t="n">
         <f aca="false">D10+E9</f>
@@ -410,7 +413,7 @@
       </c>
       <c r="C11" s="0" t="n">
         <f aca="false">B11+C10</f>
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E11" s="0" t="n">
         <f aca="false">D11+E10</f>
@@ -431,7 +434,7 @@
       </c>
       <c r="C12" s="0" t="n">
         <f aca="false">B12+C11</f>
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E12" s="0" t="n">
         <f aca="false">D12+E11</f>
@@ -452,7 +455,7 @@
       </c>
       <c r="C13" s="0" t="n">
         <f aca="false">B13+C12</f>
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E13" s="0" t="n">
         <f aca="false">D13+E12</f>

</xml_diff>

<commit_message>
Hours - Patrick and Mike
Updated hours for patrick and mike
</commit_message>
<xml_diff>
--- a/Time Sheet.xlsx
+++ b/Time Sheet.xlsx
@@ -174,7 +174,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -359,18 +359,18 @@
         <v>27</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="E8" s="0" t="n">
         <f aca="false">D8+E7</f>
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="F8" s="0" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="G8" s="0" t="n">
         <f aca="false">F8+G7</f>
-        <v>46.5</v>
+        <v>53.5</v>
       </c>
       <c r="I8" s="0" t="n">
         <f aca="false">H8</f>
@@ -385,13 +385,19 @@
         <f aca="false">B9+C8</f>
         <v>27</v>
       </c>
+      <c r="D9" s="0" t="n">
+        <v>16</v>
+      </c>
       <c r="E9" s="0" t="n">
         <f aca="false">D9+E8</f>
-        <v>60</v>
+        <v>87</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>15</v>
       </c>
       <c r="G9" s="0" t="n">
         <f aca="false">F9 +G8</f>
-        <v>46.5</v>
+        <v>68.5</v>
       </c>
       <c r="I9" s="0" t="n">
         <f aca="false">H9</f>
@@ -408,11 +414,11 @@
       </c>
       <c r="E10" s="0" t="n">
         <f aca="false">D10+E9</f>
-        <v>60</v>
+        <v>87</v>
       </c>
       <c r="G10" s="0" t="n">
         <f aca="false">F10 +G9</f>
-        <v>46.5</v>
+        <v>68.5</v>
       </c>
       <c r="I10" s="0" t="n">
         <f aca="false">H10</f>
@@ -429,11 +435,11 @@
       </c>
       <c r="E11" s="0" t="n">
         <f aca="false">D11+E10</f>
-        <v>60</v>
+        <v>87</v>
       </c>
       <c r="G11" s="0" t="n">
         <f aca="false">F11+G10</f>
-        <v>46.5</v>
+        <v>68.5</v>
       </c>
       <c r="I11" s="0" t="n">
         <f aca="false">H11</f>
@@ -450,11 +456,11 @@
       </c>
       <c r="E12" s="0" t="n">
         <f aca="false">D12+E11</f>
-        <v>60</v>
+        <v>87</v>
       </c>
       <c r="G12" s="0" t="n">
         <f aca="false">F12+G11</f>
-        <v>46.5</v>
+        <v>68.5</v>
       </c>
       <c r="I12" s="0" t="n">
         <f aca="false">H12</f>
@@ -471,11 +477,11 @@
       </c>
       <c r="E13" s="0" t="n">
         <f aca="false">D13+E12</f>
-        <v>60</v>
+        <v>87</v>
       </c>
       <c r="G13" s="0" t="n">
         <f aca="false">F13+G12</f>
-        <v>46.5</v>
+        <v>68.5</v>
       </c>
       <c r="I13" s="0" t="n">
         <f aca="false">H13</f>

</xml_diff>

<commit_message>
updated times mike and patrick
</commit_message>
<xml_diff>
--- a/Time Sheet.xlsx
+++ b/Time Sheet.xlsx
@@ -174,7 +174,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -446,18 +446,18 @@
         <v>49</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="E11" s="0" t="n">
         <f aca="false">D11+E10</f>
-        <v>118</v>
+        <v>130</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="G11" s="0" t="n">
         <f aca="false">F11+G10</f>
-        <v>96.5</v>
+        <v>102.5</v>
       </c>
       <c r="I11" s="0" t="n">
         <f aca="false">H11</f>
@@ -472,13 +472,16 @@
         <f aca="false">B12+C11</f>
         <v>49</v>
       </c>
+      <c r="D12" s="0" t="n">
+        <v>12</v>
+      </c>
       <c r="E12" s="0" t="n">
         <f aca="false">D12+E11</f>
-        <v>118</v>
+        <v>142</v>
       </c>
       <c r="G12" s="0" t="n">
         <f aca="false">F12+G11</f>
-        <v>96.5</v>
+        <v>102.5</v>
       </c>
       <c r="I12" s="0" t="n">
         <f aca="false">H12</f>
@@ -495,11 +498,11 @@
       </c>
       <c r="E13" s="0" t="n">
         <f aca="false">D13+E12</f>
-        <v>118</v>
+        <v>142</v>
       </c>
       <c r="G13" s="0" t="n">
         <f aca="false">F13+G12</f>
-        <v>96.5</v>
+        <v>102.5</v>
       </c>
       <c r="I13" s="0" t="n">
         <f aca="false">H13</f>

</xml_diff>

<commit_message>
Updated hours (all team)
</commit_message>
<xml_diff>
--- a/Time Sheet.xlsx
+++ b/Time Sheet.xlsx
@@ -174,7 +174,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -482,15 +482,18 @@
         <v>86</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E12" s="0" t="n">
         <f aca="false">D12+E11</f>
-        <v>142</v>
+        <v>146</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>14</v>
       </c>
       <c r="G12" s="0" t="n">
         <f aca="false">F12+G11</f>
-        <v>102.5</v>
+        <v>116.5</v>
       </c>
       <c r="I12" s="0" t="n">
         <f aca="false">H12</f>
@@ -501,17 +504,26 @@
       <c r="A13" s="0" t="s">
         <v>17</v>
       </c>
+      <c r="B13" s="0" t="n">
+        <v>30</v>
+      </c>
       <c r="C13" s="0" t="n">
         <f aca="false">B13+C12</f>
-        <v>86</v>
+        <v>116</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>28</v>
       </c>
       <c r="E13" s="0" t="n">
         <f aca="false">D13+E12</f>
-        <v>142</v>
+        <v>174</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>15</v>
       </c>
       <c r="G13" s="0" t="n">
         <f aca="false">F13+G12</f>
-        <v>102.5</v>
+        <v>131.5</v>
       </c>
       <c r="I13" s="0" t="n">
         <f aca="false">H13</f>

</xml_diff>